<commit_message>
updated count after replacement for weldment
</commit_message>
<xml_diff>
--- a/backend/uploads/cost-weldment-copy.xlsx
+++ b/backend/uploads/cost-weldment-copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vedan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CDE618-868D-43D7-AE03-1A5284C5235B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88BCCDF-86CB-4BA0-A304-2991D8A0C871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70C08E72-D1C2-4795-BEC7-AFB1E5DA6AF6}"/>
   </bookViews>
@@ -185,7 +185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +201,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -303,6 +309,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -713,7 +725,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="L11" sqref="L11:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1144,10 +1156,10 @@
       <c r="K11" s="12">
         <v>40.6</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="18">
         <v>185.14</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="19">
         <v>9</v>
       </c>
     </row>
@@ -1185,10 +1197,10 @@
       <c r="K12" s="12">
         <v>40.6</v>
       </c>
-      <c r="L12" s="17">
+      <c r="L12" s="18">
         <v>184.31</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M12" s="19">
         <v>115</v>
       </c>
     </row>

</xml_diff>